<commit_message>
Add Test github push
</commit_message>
<xml_diff>
--- a/Projecten/Projecten_Lopend/Project RGB/Agenda/Vergadering documentatie/Notulen_Actie_en_Besluitenlijst.xlsx
+++ b/Projecten/Projecten_Lopend/Project RGB/Agenda/Vergadering documentatie/Notulen_Actie_en_Besluitenlijst.xlsx
@@ -1726,7 +1726,9 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <Aantal xmlns="e5014122-0f0a-4a7a-8043-8075ae17fa9b">1</Aantal>
+  </documentManagement>
 </p:properties>
 </file>
 
@@ -1740,8 +1742,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B6045094B2337B4E861EE53AF1B18597" ma:contentTypeVersion="9" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="fcd73eb9399bf964593a2c5968538bf5">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e5014122-0f0a-4a7a-8043-8075ae17fa9b" xmlns:ns3="650060f8-5ca3-4039-8c45-fe2a2bb4b312" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c23a18aec2a3fb4a4b196e30e21d7de9" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B6045094B2337B4E861EE53AF1B18597" ma:contentTypeVersion="11" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="dc843967ebd8ea9a9aabe7a53e08e0d9">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e5014122-0f0a-4a7a-8043-8075ae17fa9b" xmlns:ns3="650060f8-5ca3-4039-8c45-fe2a2bb4b312" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fca66ed923399070d37c96f0adc8a4a6" ns2:_="" ns3:_="">
     <xsd:import namespace="e5014122-0f0a-4a7a-8043-8075ae17fa9b"/>
     <xsd:import namespace="650060f8-5ca3-4039-8c45-fe2a2bb4b312"/>
     <xsd:element name="properties">
@@ -1759,6 +1761,8 @@
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:Aantal" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1804,6 +1808,16 @@
     <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Aantal" ma:index="18" nillable="true" ma:displayName="Aantal" ma:default="1" ma:format="Dropdown" ma:internalName="Aantal" ma:percentage="FALSE">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Number"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1945,5 +1959,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{367A4BD4-89C8-49A7-B2E9-804187353FCD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E052792-6BFE-49B4-BD5E-949DB9C4AC15}"/>
 </file>
</xml_diff>